<commit_message>
Continuando con la memoria (Bagging)...
</commit_message>
<xml_diff>
--- a/excel_modelos.xlsx
+++ b/excel_modelos.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alberto/UCM/Machine Learning/Practica ML/MachineLearning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A690288C-87EE-024B-B3DE-9C8E7EC6077A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43FFDA6A-C188-0B43-A276-A4D01A0CBE9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16340" xr2:uid="{B0840C7C-E82D-0F46-8C15-AC9C71E25BFA}"/>
+    <workbookView xWindow="5260" yWindow="-16500" windowWidth="28040" windowHeight="16340" activeTab="2" xr2:uid="{B0840C7C-E82D-0F46-8C15-AC9C71E25BFA}"/>
   </bookViews>
   <sheets>
     <sheet name="avnnet" sheetId="1" r:id="rId1"/>
+    <sheet name="modelo1" sheetId="2" r:id="rId2"/>
+    <sheet name="modelo2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">avnnet!#REF!</definedName>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="216">
   <si>
     <t>size</t>
   </si>
@@ -1046,8 +1048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DC396EB-C8BA-6C4F-BE4D-4CBA37822C79}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="92" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:E20"/>
+    <sheetView topLeftCell="A23" zoomScaleNormal="92" workbookViewId="0">
+      <selection activeCell="E28" sqref="A28:E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1718,21 +1720,6 @@
       <c r="H27" s="2"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="F28" s="2" t="s">
         <v>4</v>
       </c>
@@ -1744,21 +1731,6 @@
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" s="1">
-        <v>10</v>
-      </c>
-      <c r="B29" s="1">
-        <v>20</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="F29" s="1" t="s">
         <v>145</v>
       </c>
@@ -1770,21 +1742,6 @@
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
-        <v>19</v>
-      </c>
-      <c r="B30" s="2">
-        <v>35</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>180</v>
-      </c>
       <c r="F30" s="2" t="s">
         <v>181</v>
       </c>
@@ -1796,21 +1753,6 @@
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A31" s="1">
-        <v>13</v>
-      </c>
-      <c r="B31" s="1">
-        <v>25</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="F31" s="1" t="s">
         <v>157</v>
       </c>
@@ -1822,21 +1764,6 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>16</v>
-      </c>
-      <c r="B32" s="1">
-        <v>30</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>168</v>
-      </c>
       <c r="F32" s="1" t="s">
         <v>169</v>
       </c>
@@ -1847,22 +1774,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
-        <v>14</v>
-      </c>
-      <c r="B33" s="2">
-        <v>25</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>160</v>
-      </c>
+    <row r="33" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F33" s="2" t="s">
         <v>161</v>
       </c>
@@ -1873,22 +1785,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
-        <v>17</v>
-      </c>
-      <c r="B34" s="2">
-        <v>30</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>172</v>
-      </c>
+    <row r="34" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F34" s="2" t="s">
         <v>173</v>
       </c>
@@ -1899,22 +1796,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A35" s="1">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1">
-        <v>15</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>132</v>
-      </c>
+    <row r="35" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F35" s="1" t="s">
         <v>133</v>
       </c>
@@ -1925,22 +1807,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
-        <v>25</v>
-      </c>
-      <c r="B36" s="2">
-        <v>45</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>204</v>
-      </c>
+    <row r="36" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F36" s="2" t="s">
         <v>205</v>
       </c>
@@ -1951,22 +1818,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
-        <v>11</v>
-      </c>
-      <c r="B37" s="2">
-        <v>20</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>148</v>
-      </c>
+    <row r="37" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F37" s="2" t="s">
         <v>149</v>
       </c>
@@ -1977,22 +1829,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
-        <v>26</v>
-      </c>
-      <c r="B38" s="2">
-        <v>45</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>208</v>
-      </c>
+    <row r="38" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F38" s="2" t="s">
         <v>209</v>
       </c>
@@ -2003,22 +1840,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
-        <v>22</v>
-      </c>
-      <c r="B39" s="2">
-        <v>40</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>192</v>
-      </c>
+    <row r="39" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F39" s="2" t="s">
         <v>193</v>
       </c>
@@ -2029,22 +1851,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>8</v>
-      </c>
-      <c r="B40" s="1">
-        <v>15</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>136</v>
-      </c>
+    <row r="40" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F40" s="1" t="s">
         <v>137</v>
       </c>
@@ -2055,22 +1862,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
-        <v>20</v>
-      </c>
-      <c r="B41" s="2">
-        <v>35</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>184</v>
-      </c>
+    <row r="41" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F41" s="2" t="s">
         <v>185</v>
       </c>
@@ -2081,22 +1873,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
-        <v>23</v>
-      </c>
-      <c r="B42" s="2">
-        <v>40</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>196</v>
-      </c>
+    <row r="42" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F42" s="2" t="s">
         <v>197</v>
       </c>
@@ -2107,22 +1884,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A43" s="1">
-        <v>5</v>
-      </c>
-      <c r="B43" s="1">
-        <v>10</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>124</v>
-      </c>
+    <row r="43" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F43" s="1" t="s">
         <v>125</v>
       </c>
@@ -2133,22 +1895,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
-        <v>4</v>
-      </c>
-      <c r="B44" s="2">
-        <v>10</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="2" t="s">
-        <v>120</v>
-      </c>
+    <row r="44" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F44" s="2" t="s">
         <v>121</v>
       </c>
@@ -2159,22 +1906,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
-        <v>15</v>
-      </c>
-      <c r="B45" s="2">
-        <v>25</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>164</v>
-      </c>
+    <row r="45" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F45" s="2" t="s">
         <v>165</v>
       </c>
@@ -2185,22 +1917,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
-        <v>24</v>
-      </c>
-      <c r="B46" s="2">
-        <v>40</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>200</v>
-      </c>
+    <row r="46" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F46" s="2" t="s">
         <v>201</v>
       </c>
@@ -2211,22 +1928,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
-        <v>12</v>
-      </c>
-      <c r="B47" s="2">
-        <v>20</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D47" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>152</v>
-      </c>
+    <row r="47" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F47" s="2" t="s">
         <v>153</v>
       </c>
@@ -2237,22 +1939,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
-        <v>21</v>
-      </c>
-      <c r="B48" s="2">
-        <v>35</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>188</v>
-      </c>
+    <row r="48" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F48" s="2" t="s">
         <v>189</v>
       </c>
@@ -2263,22 +1950,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
-        <v>18</v>
-      </c>
-      <c r="B49" s="2">
-        <v>30</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E49" s="2" t="s">
-        <v>176</v>
-      </c>
+    <row r="49" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F49" s="2" t="s">
         <v>177</v>
       </c>
@@ -2289,22 +1961,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
-        <v>27</v>
-      </c>
-      <c r="B50" s="2">
-        <v>45</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E50" s="2" t="s">
-        <v>212</v>
-      </c>
+    <row r="50" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F50" s="2" t="s">
         <v>213</v>
       </c>
@@ -2315,22 +1972,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
-        <v>9</v>
-      </c>
-      <c r="B51" s="2">
-        <v>15</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E51" s="2" t="s">
-        <v>140</v>
-      </c>
+    <row r="51" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F51" s="2" t="s">
         <v>141</v>
       </c>
@@ -2341,22 +1983,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
-        <v>6</v>
-      </c>
-      <c r="B52" s="2">
-        <v>10</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D52" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E52" s="2" t="s">
-        <v>128</v>
-      </c>
+    <row r="52" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F52" s="2" t="s">
         <v>129</v>
       </c>
@@ -2367,22 +1994,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
-        <v>2</v>
-      </c>
-      <c r="B53" s="2">
-        <v>5</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="2" t="s">
-        <v>112</v>
-      </c>
+    <row r="53" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F53" s="2" t="s">
         <v>113</v>
       </c>
@@ -2393,22 +2005,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
-        <v>1</v>
-      </c>
-      <c r="B54" s="2">
-        <v>5</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>108</v>
-      </c>
+    <row r="54" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F54" s="2" t="s">
         <v>109</v>
       </c>
@@ -2419,22 +2016,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
-        <v>3</v>
-      </c>
-      <c r="B55" s="2">
-        <v>5</v>
-      </c>
-      <c r="C55" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>116</v>
-      </c>
+    <row r="55" spans="6:8" x14ac:dyDescent="0.2">
       <c r="F55" s="2" t="s">
         <v>117</v>
       </c>
@@ -2446,11 +2028,778 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A28:H28" xr:uid="{3614577C-0E50-2A41-93FB-65D835B74EE4}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A29:H55">
-      <sortCondition descending="1" ref="E28:E55"/>
-    </sortState>
-  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{964C7671-A2D1-4142-9EF5-E6CE4609B35C}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1">
+        <v>25</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1">
+        <v>40</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>13</v>
+      </c>
+      <c r="B8">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
+        <v>15</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>20</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>40</v>
+      </c>
+      <c r="C17" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>9</v>
+      </c>
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19">
+        <v>15</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>5</v>
+      </c>
+      <c r="B20">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>6</v>
+      </c>
+      <c r="B21">
+        <v>10</v>
+      </c>
+      <c r="C21" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="B22">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23">
+        <v>5</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551935DF-0266-8A48-9689-8D2672101205}">
+  <dimension ref="A1:D28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>35</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>30</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>30</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>15</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>45</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2">
+        <v>45</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>40</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>15</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>35</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2">
+        <v>40</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2">
+        <v>10</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2">
+        <v>25</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2">
+        <v>40</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2">
+        <v>20</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2">
+        <v>35</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2">
+        <v>30</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2">
+        <v>45</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2">
+        <v>15</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2">
+        <v>10</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2">
+        <v>5</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" s="2">
+        <v>5</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>